<commit_message>
Test adaptados al modelo
</commit_message>
<xml_diff>
--- a/censuses_1b/src/test/resources/censo_incorrecto.xlsx
+++ b/censuses_1b/src/test/resources/censo_incorrecto.xlsx
@@ -427,7 +427,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,9 +479,6 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
@@ -501,9 +498,6 @@
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
@@ -519,9 +513,6 @@
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>